<commit_message>
fix export supplier info
</commit_message>
<xml_diff>
--- a/app/webroot/img/purchasing/suppliers.xlsx
+++ b/app/webroot/img/purchasing/suppliers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="21075" windowHeight="10035"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="20610" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>KOUFU PACKAGING CORP</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>Emails</t>
+  </si>
+  <si>
+    <t>Contact #</t>
   </si>
 </sst>
 </file>
@@ -62,7 +65,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -70,13 +73,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -380,39 +419,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="56" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="7"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>